<commit_message>
MathSelfEfficacy was somehow rounded incorrectly.
</commit_message>
<xml_diff>
--- a/MathSelfEfficacy/MathSelfEfficacy.xlsx
+++ b/MathSelfEfficacy/MathSelfEfficacy.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="168">
   <si>
     <t>Gender</t>
   </si>
@@ -23,6 +23,9 @@
     <t>ConfidenceRatingMean</t>
   </si>
   <si>
+    <t>Comments</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -444,6 +447,75 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Shane Goodwin and other researchers studied factors that affect a student's confidence</t>
+  </si>
+  <si>
+    <t>on a multiple-choice Mathematics exam. A group of n = 139 students in an Intermediate</t>
+  </si>
+  <si>
+    <t>Algebra course at BYU-Idaho participated in the study.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>The exam consisted of 30 multiple-choice problems worth a total of 100 points.</t>
+  </si>
+  <si>
+    <t>The students' scores out of 100 points are given in the variable "Scores."</t>
+  </si>
+  <si>
+    <t>For each test question, the students evaluated their confidence in their response</t>
+  </si>
+  <si>
+    <t>on a scale of 1 to 6.</t>
+  </si>
+  <si>
+    <t>Confidence Rating Scale:</t>
+  </si>
+  <si>
+    <t>1 - Random guess (no clue)</t>
+  </si>
+  <si>
+    <t>2 - Very unsure</t>
+  </si>
+  <si>
+    <t>3 - Somewhat unsure</t>
+  </si>
+  <si>
+    <t>4 - Somewhat sure</t>
+  </si>
+  <si>
+    <t>5 - Very sure</t>
+  </si>
+  <si>
+    <t>6 - Certain (absolutely sure)</t>
+  </si>
+  <si>
+    <t>Confidence ratings were not relayed to the instructor, and they did not affect the grade</t>
+  </si>
+  <si>
+    <t>on the exam.</t>
+  </si>
+  <si>
+    <t>The mean confidence rating marked by each student is given in the variable</t>
+  </si>
+  <si>
+    <t>"ConfidenceRatingMean."</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>K. Shane Goodwin, Lee Ostrom, and Karen Wilson Scott. Gender differences in</t>
+  </si>
+  <si>
+    <t>mathematics self-efficacy and back substitution in multiple-choice assessment.</t>
+  </si>
+  <si>
+    <t>Journal of Adult Education, 38(1):22-42, 2009.</t>
   </si>
 </sst>
 </file>
@@ -505,13 +577,16 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" t="n">
         <v>50.0</v>
@@ -519,41 +594,50 @@
       <c r="D2" t="n">
         <v>4.34</v>
       </c>
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C3" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D3" t="n">
         <v>4.73</v>
       </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C4" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D4" t="n">
         <v>5.28</v>
       </c>
+      <c r="E4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C5" t="n">
         <v>50.0</v>
@@ -561,41 +645,50 @@
       <c r="D5" t="n">
         <v>2.83</v>
       </c>
+      <c r="E5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C6" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D6" t="n">
         <v>5.4</v>
       </c>
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C7" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D7" t="n">
         <v>4.03</v>
       </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C8" t="n">
         <v>100.0</v>
@@ -603,41 +696,50 @@
       <c r="D8" t="n">
         <v>4.9</v>
       </c>
+      <c r="E8" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C9" t="n">
-        <v>97.0</v>
+        <v>96.7</v>
       </c>
       <c r="D9" t="n">
         <v>5.93</v>
       </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C10" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D10" t="n">
         <v>3.89</v>
       </c>
+      <c r="E10" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C11" t="n">
         <v>60.0</v>
@@ -645,13 +747,16 @@
       <c r="D11" t="n">
         <v>2.48</v>
       </c>
+      <c r="E11" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C12" t="n">
         <v>70.0</v>
@@ -659,13 +764,16 @@
       <c r="D12" t="n">
         <v>3.53</v>
       </c>
+      <c r="E12" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C13" t="n">
         <v>90.0</v>
@@ -673,41 +781,50 @@
       <c r="D13" t="n">
         <v>5.27</v>
       </c>
+      <c r="E13" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C14" t="n">
-        <v>33.0</v>
+        <v>33.3</v>
       </c>
       <c r="D14" t="n">
         <v>2.37</v>
       </c>
+      <c r="E14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C15" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D15" t="n">
         <v>4.31</v>
       </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C16" t="n">
         <v>80.0</v>
@@ -715,139 +832,169 @@
       <c r="D16" t="n">
         <v>5.33</v>
       </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C17" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D17" t="n">
         <v>4.13</v>
       </c>
+      <c r="E17" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C18" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D18" t="n">
         <v>5.7</v>
       </c>
+      <c r="E18" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C19" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D19" t="n">
         <v>5.17</v>
       </c>
+      <c r="E19" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C20" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D20" t="n">
         <v>4.33</v>
       </c>
+      <c r="E20" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C21" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D21" t="n">
         <v>5.33</v>
       </c>
+      <c r="E21" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C22" t="n">
-        <v>63.0</v>
+        <v>63.3</v>
       </c>
       <c r="D22" t="n">
         <v>3.83</v>
       </c>
+      <c r="E22" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C23" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D23" t="n">
         <v>4.93</v>
       </c>
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C24" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D24" t="n">
         <v>4.57</v>
       </c>
+      <c r="E24" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C25" t="n">
-        <v>47.0</v>
+        <v>46.7</v>
       </c>
       <c r="D25" t="n">
         <v>4.07</v>
       </c>
+      <c r="E25" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C26" t="n">
         <v>70.0</v>
@@ -855,13 +1002,16 @@
       <c r="D26" t="n">
         <v>3.37</v>
       </c>
+      <c r="E26" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C27" t="n">
         <v>80.0</v>
@@ -869,27 +1019,33 @@
       <c r="D27" t="n">
         <v>4.4</v>
       </c>
+      <c r="E27" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C28" t="n">
-        <v>43.0</v>
+        <v>43.3</v>
       </c>
       <c r="D28" t="n">
         <v>2.0</v>
       </c>
+      <c r="E28" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" t="n">
         <v>60.0</v>
@@ -897,13 +1053,16 @@
       <c r="D29" t="n">
         <v>3.57</v>
       </c>
+      <c r="E29" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C30" t="n">
         <v>80.0</v>
@@ -911,13 +1070,16 @@
       <c r="D30" t="n">
         <v>4.6</v>
       </c>
+      <c r="E30" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C31" t="n">
         <v>50.0</v>
@@ -925,13 +1087,16 @@
       <c r="D31" t="n">
         <v>3.4</v>
       </c>
+      <c r="E31" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C32" t="n">
         <v>80.0</v>
@@ -939,27 +1104,33 @@
       <c r="D32" t="n">
         <v>3.72</v>
       </c>
+      <c r="E32" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C33" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D33" t="n">
         <v>4.14</v>
       </c>
+      <c r="E33" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C34" t="n">
         <v>90.0</v>
@@ -967,55 +1138,67 @@
       <c r="D34" t="n">
         <v>4.17</v>
       </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C35" t="n">
-        <v>97.0</v>
+        <v>96.7</v>
       </c>
       <c r="D35" t="n">
         <v>4.3</v>
       </c>
+      <c r="E35" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C36" t="n">
-        <v>53.0</v>
+        <v>53.3</v>
       </c>
       <c r="D36" t="n">
         <v>2.35</v>
       </c>
+      <c r="E36" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C37" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D37" t="n">
         <v>4.63</v>
       </c>
+      <c r="E37" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C38" t="n">
         <v>30.0</v>
@@ -1023,41 +1206,50 @@
       <c r="D38" t="n">
         <v>3.9</v>
       </c>
+      <c r="E38" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C39" t="n">
-        <v>53.0</v>
+        <v>53.3</v>
       </c>
       <c r="D39" t="n">
         <v>3.73</v>
       </c>
+      <c r="E39" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C40" t="n">
-        <v>67.0</v>
+        <v>66.7</v>
       </c>
       <c r="D40" t="n">
         <v>4.43</v>
       </c>
+      <c r="E40" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C41" t="n">
         <v>100.0</v>
@@ -1065,27 +1257,33 @@
       <c r="D41" t="n">
         <v>5.53</v>
       </c>
+      <c r="E41" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C42" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D42" t="n">
         <v>5.43</v>
       </c>
+      <c r="E42" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C43" t="n">
         <v>90.0</v>
@@ -1093,27 +1291,33 @@
       <c r="D43" t="n">
         <v>4.37</v>
       </c>
+      <c r="E43" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C44" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D44" t="n">
         <v>3.8</v>
       </c>
+      <c r="E44" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C45" t="n">
         <v>90.0</v>
@@ -1121,27 +1325,33 @@
       <c r="D45" t="n">
         <v>4.73</v>
       </c>
+      <c r="E45" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C46" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D46" t="n">
         <v>4.69</v>
       </c>
+      <c r="E46" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C47" t="n">
         <v>70.0</v>
@@ -1149,125 +1359,152 @@
       <c r="D47" t="n">
         <v>4.13</v>
       </c>
+      <c r="E47" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C48" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D48" t="n">
         <v>5.3</v>
       </c>
+      <c r="E48" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C49" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D49" t="n">
         <v>5.03</v>
       </c>
+      <c r="E49" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C50" t="n">
-        <v>67.0</v>
+        <v>66.7</v>
       </c>
       <c r="D50" t="n">
         <v>3.79</v>
       </c>
+      <c r="E50" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C51" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D51" t="n">
         <v>4.47</v>
       </c>
+      <c r="E51" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C52" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D52" t="n">
         <v>4.47</v>
       </c>
+      <c r="E52" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C53" t="n">
-        <v>47.0</v>
+        <v>46.7</v>
       </c>
       <c r="D53" t="n">
         <v>2.77</v>
       </c>
+      <c r="E53" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C54" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D54" t="n">
         <v>4.2</v>
       </c>
+      <c r="E54" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C55" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D55" t="n">
         <v>5.33</v>
       </c>
+      <c r="E55" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C56" t="n">
         <v>70.0</v>
@@ -1275,13 +1512,16 @@
       <c r="D56" t="n">
         <v>3.83</v>
       </c>
+      <c r="E56" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C57" t="n">
         <v>100.0</v>
@@ -1289,13 +1529,16 @@
       <c r="D57" t="n">
         <v>5.5</v>
       </c>
+      <c r="E57" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C58" t="n">
         <v>50.0</v>
@@ -1303,13 +1546,16 @@
       <c r="D58" t="n">
         <v>4.67</v>
       </c>
+      <c r="E58" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C59" t="n">
         <v>80.0</v>
@@ -1317,13 +1563,16 @@
       <c r="D59" t="n">
         <v>5.13</v>
       </c>
+      <c r="E59" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C60" t="n">
         <v>70.0</v>
@@ -1331,97 +1580,118 @@
       <c r="D60" t="n">
         <v>4.5</v>
       </c>
+      <c r="E60" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C61" t="n">
-        <v>97.0</v>
+        <v>96.7</v>
       </c>
       <c r="D61" t="n">
         <v>5.5</v>
       </c>
+      <c r="E61" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C62" t="n">
-        <v>47.0</v>
+        <v>46.7</v>
       </c>
       <c r="D62" t="n">
         <v>3.21</v>
       </c>
+      <c r="E62" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C63" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D63" t="n">
         <v>5.5</v>
       </c>
+      <c r="E63" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C64" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D64" t="n">
         <v>4.37</v>
       </c>
+      <c r="E64" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C65" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D65" t="n">
         <v>4.11</v>
       </c>
+      <c r="E65" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C66" t="n">
-        <v>53.0</v>
+        <v>53.3</v>
       </c>
       <c r="D66" t="n">
         <v>4.17</v>
       </c>
+      <c r="E66" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C67" t="n">
         <v>70.0</v>
@@ -1429,13 +1699,16 @@
       <c r="D67" t="n">
         <v>4.12</v>
       </c>
+      <c r="E67" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C68" t="n">
         <v>90.0</v>
@@ -1443,55 +1716,67 @@
       <c r="D68" t="n">
         <v>4.7</v>
       </c>
+      <c r="E68" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C69" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D69" t="n">
         <v>5.0</v>
       </c>
+      <c r="E69" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C70" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D70" t="n">
         <v>5.41</v>
       </c>
+      <c r="E70" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C71" t="n">
-        <v>63.0</v>
+        <v>63.3</v>
       </c>
       <c r="D71" t="n">
         <v>3.03</v>
       </c>
+      <c r="E71" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C72" t="n">
         <v>50.0</v>
@@ -1499,13 +1784,16 @@
       <c r="D72" t="n">
         <v>3.47</v>
       </c>
+      <c r="E72" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C73" t="n">
         <v>60.0</v>
@@ -1513,111 +1801,135 @@
       <c r="D73" t="n">
         <v>1.57</v>
       </c>
+      <c r="E73" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C74" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D74" t="n">
         <v>3.2</v>
       </c>
+      <c r="E74" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C75" t="n">
-        <v>37.0</v>
+        <v>36.7</v>
       </c>
       <c r="D75" t="n">
         <v>3.0</v>
       </c>
+      <c r="E75" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C76" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D76" t="n">
         <v>5.67</v>
       </c>
+      <c r="E76" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C77" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D77" t="n">
         <v>4.43</v>
       </c>
+      <c r="E77" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C78" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D78" t="n">
         <v>5.1</v>
       </c>
+      <c r="E78" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C79" t="n">
-        <v>57.0</v>
+        <v>56.7</v>
       </c>
       <c r="D79" t="n">
         <v>3.28</v>
       </c>
+      <c r="E79" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C80" t="n">
-        <v>97.0</v>
+        <v>96.7</v>
       </c>
       <c r="D80" t="n">
         <v>6.0</v>
       </c>
+      <c r="E80" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C81" t="n">
         <v>70.0</v>
@@ -1625,69 +1937,84 @@
       <c r="D81" t="n">
         <v>5.4</v>
       </c>
+      <c r="E81" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C82" t="n">
-        <v>67.0</v>
+        <v>66.7</v>
       </c>
       <c r="D82" t="n">
         <v>3.9</v>
       </c>
+      <c r="E82" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C83" t="n">
-        <v>67.0</v>
+        <v>66.7</v>
       </c>
       <c r="D83" t="n">
         <v>3.67</v>
       </c>
+      <c r="E83" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C84" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D84" t="n">
         <v>4.33</v>
       </c>
+      <c r="E84" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C85" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D85" t="n">
         <v>5.87</v>
       </c>
+      <c r="E85" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C86" t="n">
         <v>90.0</v>
@@ -1695,181 +2022,220 @@
       <c r="D86" t="n">
         <v>5.31</v>
       </c>
+      <c r="E86" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C87" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D87" t="n">
         <v>4.6</v>
       </c>
+      <c r="E87" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C88" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D88" t="n">
         <v>5.97</v>
       </c>
+      <c r="E88" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C89" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D89" t="n">
         <v>4.27</v>
       </c>
+      <c r="E89" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C90" t="n">
-        <v>43.0</v>
+        <v>43.3</v>
       </c>
       <c r="D90" t="n">
         <v>4.56</v>
       </c>
+      <c r="E90" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C91" t="n">
-        <v>63.0</v>
+        <v>63.3</v>
       </c>
       <c r="D91" t="n">
         <v>4.23</v>
       </c>
+      <c r="E91" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C92" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D92" t="n">
         <v>4.9</v>
       </c>
+      <c r="E92" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C93" t="n">
-        <v>67.0</v>
+        <v>66.7</v>
       </c>
       <c r="D93" t="n">
         <v>4.83</v>
       </c>
+      <c r="E93" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C94" t="n">
-        <v>57.0</v>
+        <v>56.7</v>
       </c>
       <c r="D94" t="n">
         <v>2.52</v>
       </c>
+      <c r="E94" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C95" t="n">
-        <v>57.0</v>
+        <v>56.7</v>
       </c>
       <c r="D95" t="n">
         <v>4.59</v>
       </c>
+      <c r="E95" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C96" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D96" t="n">
         <v>3.12</v>
       </c>
+      <c r="E96" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C97" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D97" t="n">
         <v>5.77</v>
       </c>
+      <c r="E97" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C98" t="n">
-        <v>67.0</v>
+        <v>66.7</v>
       </c>
       <c r="D98" t="n">
         <v>4.43</v>
       </c>
+      <c r="E98" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C99" t="n">
         <v>100.0</v>
@@ -1877,69 +2243,84 @@
       <c r="D99" t="n">
         <v>5.2</v>
       </c>
+      <c r="E99" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C100" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D100" t="n">
         <v>5.6</v>
       </c>
+      <c r="E100" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C101" t="n">
-        <v>43.0</v>
+        <v>43.3</v>
       </c>
       <c r="D101" t="n">
         <v>2.37</v>
       </c>
+      <c r="E101" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C102" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D102" t="n">
         <v>4.8</v>
       </c>
+      <c r="E102" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C103" t="n">
-        <v>63.0</v>
+        <v>63.3</v>
       </c>
       <c r="D103" t="n">
         <v>4.62</v>
       </c>
+      <c r="E103" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C104" t="n">
         <v>40.0</v>
@@ -1947,41 +2328,50 @@
       <c r="D104" t="n">
         <v>3.53</v>
       </c>
+      <c r="E104" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C105" t="n">
-        <v>43.0</v>
+        <v>43.3</v>
       </c>
       <c r="D105" t="n">
         <v>2.61</v>
       </c>
+      <c r="E105" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C106" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D106" t="n">
         <v>3.45</v>
       </c>
+      <c r="E106" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C107" t="n">
         <v>90.0</v>
@@ -1989,55 +2379,67 @@
       <c r="D107" t="n">
         <v>4.6</v>
       </c>
+      <c r="E107" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C108" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D108" t="n">
         <v>6.0</v>
       </c>
+      <c r="E108" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C109" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D109" t="n">
         <v>4.93</v>
       </c>
+      <c r="E109" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C110" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D110" t="n">
         <v>5.17</v>
       </c>
+      <c r="E110" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C111" t="n">
         <v>80.0</v>
@@ -2045,69 +2447,84 @@
       <c r="D111" t="n">
         <v>4.33</v>
       </c>
+      <c r="E111" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C112" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D112" t="n">
         <v>5.37</v>
       </c>
+      <c r="E112" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C113" t="n">
-        <v>53.0</v>
+        <v>53.3</v>
       </c>
       <c r="D113" t="n">
         <v>3.62</v>
       </c>
+      <c r="E113" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C114" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D114" t="n">
         <v>4.5</v>
       </c>
+      <c r="E114" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C115" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D115" t="n">
         <v>4.31</v>
       </c>
+      <c r="E115" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C116" t="n">
         <v>90.0</v>
@@ -2115,69 +2532,84 @@
       <c r="D116" t="n">
         <v>5.33</v>
       </c>
+      <c r="E116" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C117" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D117" t="n">
         <v>4.7</v>
       </c>
+      <c r="E117" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C118" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D118" t="n">
         <v>3.3</v>
       </c>
+      <c r="E118" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C119" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D119" t="n">
         <v>5.73</v>
       </c>
+      <c r="E119" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C120" t="n">
-        <v>93.0</v>
+        <v>93.3</v>
       </c>
       <c r="D120" t="n">
         <v>4.93</v>
       </c>
+      <c r="E120" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C121" t="n">
         <v>80.0</v>
@@ -2185,13 +2617,16 @@
       <c r="D121" t="n">
         <v>3.83</v>
       </c>
+      <c r="E121" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C122" t="n">
         <v>80.0</v>
@@ -2199,27 +2634,33 @@
       <c r="D122" t="n">
         <v>5.13</v>
       </c>
+      <c r="E122" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C123" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D123" t="n">
         <v>5.67</v>
       </c>
+      <c r="E123" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C124" t="n">
         <v>70.0</v>
@@ -2227,55 +2668,67 @@
       <c r="D124" t="n">
         <v>4.87</v>
       </c>
+      <c r="E124" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C125" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D125" t="n">
         <v>4.15</v>
       </c>
+      <c r="E125" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C126" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D126" t="n">
         <v>4.37</v>
       </c>
+      <c r="E126" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C127" t="n">
-        <v>57.0</v>
+        <v>56.7</v>
       </c>
       <c r="D127" t="n">
         <v>3.36</v>
       </c>
+      <c r="E127" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C128" t="n">
         <v>90.0</v>
@@ -2283,27 +2736,33 @@
       <c r="D128" t="n">
         <v>5.17</v>
       </c>
+      <c r="E128" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C129" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D129" t="n">
         <v>4.37</v>
       </c>
+      <c r="E129" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C130" t="n">
         <v>90.0</v>
@@ -2311,97 +2770,118 @@
       <c r="D130" t="n">
         <v>5.2</v>
       </c>
+      <c r="E130" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C131" t="n">
-        <v>53.0</v>
+        <v>53.3</v>
       </c>
       <c r="D131" t="n">
         <v>3.4</v>
       </c>
+      <c r="E131" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C132" t="n">
-        <v>37.0</v>
+        <v>36.7</v>
       </c>
       <c r="D132" t="n">
         <v>3.34</v>
       </c>
+      <c r="E132" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C133" t="n">
-        <v>83.0</v>
+        <v>83.3</v>
       </c>
       <c r="D133" t="n">
         <v>4.04</v>
       </c>
+      <c r="E133" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C134" t="n">
-        <v>73.0</v>
+        <v>73.3</v>
       </c>
       <c r="D134" t="n">
         <v>4.27</v>
       </c>
+      <c r="E134" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C135" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D135" t="n">
         <v>5.43</v>
       </c>
+      <c r="E135" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C136" t="n">
-        <v>87.0</v>
+        <v>86.7</v>
       </c>
       <c r="D136" t="n">
         <v>5.83</v>
       </c>
+      <c r="E136" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C137" t="n">
         <v>90.0</v>
@@ -2409,47 +2889,59 @@
       <c r="D137" t="n">
         <v>5.77</v>
       </c>
+      <c r="E137" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C138" t="n">
-        <v>97.0</v>
+        <v>96.7</v>
       </c>
       <c r="D138" t="n">
         <v>5.8</v>
       </c>
+      <c r="E138" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C139" t="n">
-        <v>77.0</v>
+        <v>76.7</v>
       </c>
       <c r="D139" t="n">
         <v>4.6</v>
       </c>
+      <c r="E139" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C140" t="n">
         <v>70.0</v>
       </c>
       <c r="D140" t="n">
         <v>3.77</v>
+      </c>
+      <c r="E140" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>